<commit_message>
Report of project status at 17.03.2023
</commit_message>
<xml_diff>
--- a/Spring Project Report .xlsx
+++ b/Spring Project Report .xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26409"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83A4781E-998F-4AB1-B083-AFDB9AC35381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2FCB9FF8-7591-4577-8D17-41F60788234F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>13.04.2023</t>
   </si>
@@ -65,13 +65,43 @@
   </si>
   <si>
     <t>Completed :)</t>
+  </si>
+  <si>
+    <t>17.04.2023</t>
+  </si>
+  <si>
+    <t>Chapter 3. Forces and Equations of Motion, Section 3.7 Hook’s Law and Simple</t>
+  </si>
+  <si>
+    <t>Youtoube videos</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=g550H4e5FCY&amp;pp=ygUeRm9yY2VzIGFuZCBFcXVhdGlvbnMgb2YgTW90aW9u</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=UNuRhIHthhY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=-_l_YDA6au8&amp;pp=ygUqNyBIb29r4oCZcyBMYXcgYW5kIFNpbXBsZSBIYXJtb25pYyBNb3Rpb24s</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=_Gnke2x3vT8&amp;pp=ygUqNyBIb29r4oCZcyBMYXcgYW5kIFNpbXBsZSBIYXJtb25pYyBNb3Rpb24s</t>
+  </si>
+  <si>
+    <t>hooke-s-law-and-simple-harmonic-motion</t>
+  </si>
+  <si>
+    <t>A_Harmonic_Oscillator_Obeys_Hooke's_Law</t>
+  </si>
+  <si>
+    <t>Task 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +116,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -109,7 +146,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -121,6 +158,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -436,7 +480,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -445,7 +489,8 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.28515625" customWidth="1"/>
+    <col min="2" max="2" width="118.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -453,8 +498,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="45.75">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:2" ht="30.75">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -462,7 +507,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -470,13 +515,13 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -484,13 +529,13 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="4"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="4"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
@@ -503,10 +548,73 @@
         <v>11</v>
       </c>
     </row>
+    <row r="10" spans="1:2">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{CFBBEA14-D424-4370-B668-A7176E6418D8}"/>
@@ -514,6 +622,12 @@
     <hyperlink ref="B5" r:id="rId3" location=":~:text=The%20simplest%20oscillations%20occur%20when,known%20as%20simple%20harmonic%20motion" xr:uid="{EFDFE842-94A8-4CF1-8714-5D57FB6D3FB5}"/>
     <hyperlink ref="B6" r:id="rId4" xr:uid="{F355E03C-40DE-4A02-8166-7436A26BB9DC}"/>
     <hyperlink ref="B7" r:id="rId5" xr:uid="{340F6686-2C76-44F6-98E9-95A6A170E0AC}"/>
+    <hyperlink ref="B13" r:id="rId6" xr:uid="{A722DCFE-9F01-4724-94E4-59B393B29E09}"/>
+    <hyperlink ref="B14" r:id="rId7" xr:uid="{5A2A89E0-9839-420E-8C1E-5346980EEB0A}"/>
+    <hyperlink ref="B15" r:id="rId8" xr:uid="{DC08F1B5-DDEE-4169-BB85-19BD9D3F29CA}"/>
+    <hyperlink ref="B16" r:id="rId9" xr:uid="{AE9F9755-664C-4ED6-83D7-204D24A66B24}"/>
+    <hyperlink ref="B17" r:id="rId10" xr:uid="{065B9D8A-4ADD-44C0-BEDA-3C84F3385BEA}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{D2B7AA6E-32C8-4615-8D4D-54587A92C8CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>